<commit_message>
Updated with smaller test size
test times only, with only one different image.
</commit_message>
<xml_diff>
--- a/Opacus MNIST comparison.xlsx
+++ b/Opacus MNIST comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Yang\Documents\Penn State Fall 2020\Honors Thesis Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750560DC-B6A4-4753-BB48-C090BB450BD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCE2878-F12D-416C-8596-7EEC435E79EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="792" yWindow="420" windowWidth="21852" windowHeight="8964" xr2:uid="{005D4E51-D04F-44E3-BC1B-7B447DA35995}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{005D4E51-D04F-44E3-BC1B-7B447DA35995}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Regular MNIST(5 epochs) - Batch 64, Test Batch 1024</t>
   </si>
@@ -37,19 +37,40 @@
   </si>
   <si>
     <t>Fashion MNIST(5 epochs) - Batch 32, Test Batch 512</t>
+  </si>
+  <si>
+    <t>MNIST, test indices [0:100], test time only</t>
+  </si>
+  <si>
+    <t>MNIST, test indices[1:101], test time only</t>
+  </si>
+  <si>
+    <t>MNIST, test indices [0:10], test time only</t>
+  </si>
+  <si>
+    <t>MNIST, test indices [1:11], test time only</t>
+  </si>
+  <si>
+    <t>python mnist.py --device=cpu -n=1 --lr=.25 --sigma=1.3 -c=1.5 -b=250</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,8 +93,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6809342-C014-4A41-B931-A50FAB80E25C}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,7 +510,125 @@
         <v>88.554500000000004</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1.8444</v>
+      </c>
+      <c r="B11">
+        <v>1.8488</v>
+      </c>
+      <c r="C11">
+        <v>1.8041</v>
+      </c>
+      <c r="D11">
+        <v>1.3995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1.4799</v>
+      </c>
+      <c r="B12">
+        <v>1.4222999999999999</v>
+      </c>
+      <c r="C12">
+        <v>1.4115</v>
+      </c>
+      <c r="D12">
+        <v>1.3873</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1.8634999999999999</v>
+      </c>
+      <c r="B13">
+        <v>1.4136</v>
+      </c>
+      <c r="C13">
+        <v>1.3996999999999999</v>
+      </c>
+      <c r="D13">
+        <v>1.3904000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1.4967999999999999</v>
+      </c>
+      <c r="B14">
+        <v>1.8388</v>
+      </c>
+      <c r="C14">
+        <v>1.3880999999999999</v>
+      </c>
+      <c r="D14">
+        <v>1.8224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1.5631999999999999</v>
+      </c>
+      <c r="B15">
+        <v>1.8508</v>
+      </c>
+      <c r="C15">
+        <v>1.8042</v>
+      </c>
+      <c r="D15">
+        <v>1.8183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1.409</v>
+      </c>
+      <c r="B16">
+        <v>1.8270999999999999</v>
+      </c>
+      <c r="C16">
+        <v>1.8561000000000001</v>
+      </c>
+      <c r="D16">
+        <v>1.8110999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1.4219999999999999</v>
+      </c>
+      <c r="B17">
+        <v>1.8409</v>
+      </c>
+      <c r="C17">
+        <v>1.3793</v>
+      </c>
+      <c r="D17">
+        <v>1.7976000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>